<commit_message>
Implemented TestStudent class, its bugged
</commit_message>
<xml_diff>
--- a/src/main/resources/projects60.xlsx
+++ b/src/main/resources/projects60.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="120">
   <si>
     <t>Supervisor</t>
   </si>
@@ -26,286 +26,307 @@
     <t>Probability</t>
   </si>
   <si>
-    <t>Phoebe Buffay</t>
-  </si>
-  <si>
-    <t>Friends and the Dagon mythos</t>
+    <t>Matt Drudge</t>
+  </si>
+  <si>
+    <t>the Right and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>CS+DS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Republicans and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> American politics and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>Pope Francis</t>
+  </si>
+  <si>
+    <t>Catholicism and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>promoting Catholic values in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Brad Pitt</t>
+  </si>
+  <si>
+    <t>Acting and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hollywood and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>starring in Hollywood movies in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Eddy Merckx</t>
+  </si>
+  <si>
+    <t>Cycling and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>pedalling furiously in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> winning cycling races in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Karl Marx</t>
+  </si>
+  <si>
+    <t>Das Capital and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Communism and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>promoting communism in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Morgana Le Fay</t>
+  </si>
+  <si>
+    <t>British history and the Dagon mythos</t>
   </si>
   <si>
     <t>DS</t>
   </si>
   <si>
-    <t>singing parody songs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> singing goofy songs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Brian Wilson</t>
-  </si>
-  <si>
-    <t>Pop music and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>CS+DS</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Love songs and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Beach Boys and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>Rihanna</t>
-  </si>
-  <si>
-    <t>Pop Music and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>CS</t>
-  </si>
-  <si>
-    <t>singing pop songs in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> writing pop songs in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Ella Fitzgerald</t>
-  </si>
-  <si>
-    <t>Music and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Jazz and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Blues music and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>Enrico Caruso</t>
-  </si>
-  <si>
-    <t>Opera and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>singing opera arias in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Cameron Diaz</t>
-  </si>
-  <si>
-    <t>Acting and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Comedy and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>starring in romantic comedies in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>William the Conqueror</t>
-  </si>
-  <si>
-    <t>British history and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>fighting with swords in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> leading armies into battle in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Norman Bates</t>
-  </si>
-  <si>
-    <t>Psycho and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hitchcock movies and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>cross-dressing in women's clothes in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Arya Stark</t>
-  </si>
-  <si>
-    <t>Game of Thrones and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Westeros and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>seeking revenge in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Greta Garbo</t>
-  </si>
-  <si>
-    <t>Hollywood and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Acting and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>starring in Hollywood movies in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Julia Child</t>
-  </si>
-  <si>
-    <t>Cooking and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Kitchen and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>cooking dinners in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Humphrey Bogart</t>
-  </si>
-  <si>
-    <t>Hollywood and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Acting and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>starring in Hollywood movies in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Joe DiMaggio</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> American sports and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Baseball and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>playing baseball in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Rain Man</t>
-  </si>
-  <si>
-    <t>Autism and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>counting tooth picks in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> counting cards in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Weird Al Yankovic</t>
-  </si>
-  <si>
-    <t>Musical Comedy and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Parody and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>singing parody songs in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Fred Astaire</t>
-  </si>
-  <si>
-    <t>Dancing and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hollywood and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>starring in romantic comedies in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Julian Assange</t>
-  </si>
-  <si>
-    <t>Espionage and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Politics and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Wikileaks and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>Tracy Jordan</t>
-  </si>
-  <si>
-    <t>30 Rock and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Television Production and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>starring in comedies in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Genghis Khan</t>
-  </si>
-  <si>
-    <t>the Mongols and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mongolia and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>running an empire in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Spider-Man</t>
+    <t>performing magic tricks in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> studying magic tricks in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Martha Stewart</t>
+  </si>
+  <si>
+    <t>Cooking and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Kitchen and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Arts and Crafts and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>Tom Sawyer</t>
+  </si>
+  <si>
+    <t>American literature and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the American South and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>playing pranks in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Savonarola</t>
+  </si>
+  <si>
+    <t>Florence and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Renaissance and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>Jane Eyre</t>
+  </si>
+  <si>
+    <t>English literature and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>looking after children in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Jay Z</t>
+  </si>
+  <si>
+    <t>Rap music and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hip-Hop and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>producing Hipbop records in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Queen Victoria</t>
+  </si>
+  <si>
+    <t>British history and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> British royalty and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>ruling over subjects in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Frank Columbo</t>
+  </si>
+  <si>
+    <t>Detective fiction and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>solving crimes in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pursuing criminals in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Edgar Allan Poe</t>
+  </si>
+  <si>
+    <t>American literature and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>writing mystery stories in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Joe Biden</t>
+  </si>
+  <si>
+    <t>the Left and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Democrats and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>plagiarizing political speeches in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Commissioner James Gordon</t>
+  </si>
+  <si>
+    <t>DC Comics and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Gotham City and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>pursuing criminals in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Shylock</t>
+  </si>
+  <si>
+    <t>Shakespeare and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>amassing wealth in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> seeking revenge in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>John Wilkes Booth</t>
+  </si>
+  <si>
+    <t>American politics and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>assassinating presidents in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>O.J. Simpson</t>
+  </si>
+  <si>
+    <t>American football and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>playing golf in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> making threatening phone calls in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Eminem</t>
+  </si>
+  <si>
+    <t>Rap music and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>writing rap songs in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Ed Wood</t>
+  </si>
+  <si>
+    <t>Bad Movies and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> B Movies and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>making bad movies in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Agent Smith</t>
+  </si>
+  <si>
+    <t>The Matrix and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>fighting the resistance in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Bridget Jones</t>
+  </si>
+  <si>
+    <t>British comedy and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> British humour and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Comedy and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>Noah</t>
+  </si>
+  <si>
+    <t>the Bible and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Old Testament and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Judaism and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>Mark Fuhrman</t>
+  </si>
+  <si>
+    <t>the Law and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Crime and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Reality TV and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>Wolverine</t>
   </si>
   <si>
     <t>Marvel Comics and the Dagon mythos</t>
   </si>
   <si>
-    <t>maintaining a secret identity in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> solving crimes in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Sean Penn</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Action movies and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> promoting social causes  in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Superman</t>
-  </si>
-  <si>
-    <t>DC Comics and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Metropolis and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The Daily Planet and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>Leo Tolstoy</t>
-  </si>
-  <si>
-    <t>Russian literature and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> War And Peace and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>writing Russian novels in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Gianni Versace</t>
+    <t xml:space="preserve"> The X-Men and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>foiling the schemes of evil villains in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Naomi Campbell</t>
   </si>
   <si>
     <t>Fashion and the Cthulu-Dagon mythos</t>
@@ -317,73 +338,40 @@
     <t xml:space="preserve"> the Fashion industry and the Cthulu-Dagon mythos</t>
   </si>
   <si>
-    <t>Rick Sanchez</t>
-  </si>
-  <si>
-    <t>Rick and Morty and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>pioneering new technologies in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> inventing electrical marvels in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>David Mamet</t>
-  </si>
-  <si>
-    <t>Movies and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Theatre and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>writing plays in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Lord Byron</t>
-  </si>
-  <si>
-    <t>English poetry and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Romantic poetry and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>writing romantic poetry in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>British history and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>fighting with swords in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> leading armies into battle in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Biff Tannen</t>
-  </si>
-  <si>
-    <t>Back To The Future and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>giving noogies in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> mangling idioms in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Princess Leia Organa</t>
-  </si>
-  <si>
-    <t>Star Wars and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>leading the rebel alliance in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> smuggling military plans in Dagon-worshipping societies</t>
+    <t>Jean-Luc Picard</t>
+  </si>
+  <si>
+    <t>Star Trek and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the U.S.S. Enterprise and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Starfleet and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>Frida Kahlo</t>
+  </si>
+  <si>
+    <t>Mexican art and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Art and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>painting colorful pictures in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>H.A.L. 9000</t>
+  </si>
+  <si>
+    <t>2001: A Space Odyssey and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Homicidal computers and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>murdering astronauts in Dagon-worshipping societies</t>
   </si>
 </sst>
 </file>
@@ -459,7 +447,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="n">
-        <v>1.4650807275492836E-5</v>
+        <v>1.5712109037655364E-5</v>
       </c>
     </row>
     <row r="3">
@@ -473,7 +461,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="n">
-        <v>2.089736706111163E-5</v>
+        <v>2.2882974782502155E-5</v>
       </c>
     </row>
     <row r="4">
@@ -487,7 +475,7 @@
         <v>6</v>
       </c>
       <c r="D4" t="n">
-        <v>2.9562069406283386E-5</v>
+        <v>3.301861938558835E-5</v>
       </c>
     </row>
     <row r="5">
@@ -501,7 +489,7 @@
         <v>11</v>
       </c>
       <c r="D5" t="n">
-        <v>4.147547224304998E-5</v>
+        <v>4.720345305784465E-5</v>
       </c>
     </row>
     <row r="6">
@@ -515,175 +503,175 @@
         <v>11</v>
       </c>
       <c r="D6" t="n">
-        <v>5.771133143082669E-5</v>
+        <v>6.685856663314933E-5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
       </c>
       <c r="D7" t="n">
-        <v>7.964235537476655E-5</v>
+        <v>9.382288586223318E-5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D8" t="n">
-        <v>1.0900347552508815E-4</v>
+        <v>1.3044545353947022E-4</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D9" t="n">
-        <v>1.4796188113642468E-4</v>
+        <v>1.7968736598590222E-4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
         <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D10" t="n">
-        <v>1.991923211064285E-4</v>
+        <v>2.4523055113574927E-4</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
         <v>19</v>
       </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D11" t="n">
-        <v>2.659552638953174E-4</v>
+        <v>3.3158894511433506E-4</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>3.5217444534218524E-4</v>
+        <v>4.4421574738256683E-4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D13" t="n">
-        <v>4.625091609729505E-4</v>
+        <v>5.895983997792394E-4</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
         <v>23</v>
       </c>
-      <c r="B14" t="s">
-        <v>24</v>
-      </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D14" t="n">
-        <v>6.024154353669231E-4</v>
+        <v>7.753308807374694E-4</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D15" t="n">
-        <v>7.781890133835537E-4</v>
+        <v>0.001010151023383744</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
         <v>26</v>
       </c>
-      <c r="B16" t="s">
-        <v>27</v>
-      </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D16" t="n">
-        <v>9.96982079153305E-4</v>
+        <v>0.001303929094273841</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
         <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0012667848535508992</v>
+        <v>0.0016675930842951102</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
         <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0015963628996320395</v>
+        <v>0.0021129763580244017</v>
       </c>
     </row>
     <row r="19">
@@ -697,7 +685,7 @@
         <v>11</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0019951412331558</v>
+        <v>0.002652574764543515</v>
       </c>
     </row>
     <row r="20">
@@ -711,7 +699,7 @@
         <v>11</v>
       </c>
       <c r="D20" t="n">
-        <v>0.0024730273370353485</v>
+        <v>0.0032992032661826737</v>
       </c>
     </row>
     <row r="21">
@@ -725,7 +713,7 @@
         <v>11</v>
       </c>
       <c r="D21" t="n">
-        <v>0.003040167032311589</v>
+        <v>0.004065546738784504</v>
       </c>
     </row>
     <row r="22">
@@ -736,10 +724,10 @@
         <v>35</v>
       </c>
       <c r="C22" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D22" t="n">
-        <v>0.0037066299353480936</v>
+        <v>0.00496360585532948</v>
       </c>
     </row>
     <row r="23">
@@ -750,10 +738,10 @@
         <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D23" t="n">
-        <v>0.00448202493663857</v>
+        <v>0.006004046735196597</v>
       </c>
     </row>
     <row r="24">
@@ -764,10 +752,10 @@
         <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D24" t="n">
-        <v>0.005375050692804178</v>
+        <v>0.007195471982361319</v>
       </c>
     </row>
     <row r="25">
@@ -781,7 +769,7 @@
         <v>6</v>
       </c>
       <c r="D25" t="n">
-        <v>0.0063929913562243805</v>
+        <v>0.008543640303901062</v>
       </c>
     </row>
     <row r="26">
@@ -795,357 +783,357 @@
         <v>6</v>
       </c>
       <c r="D26" t="n">
-        <v>0.007541173401749111</v>
+        <v>0.010050671362960006</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D27" t="n">
-        <v>0.008822405076672146</v>
+        <v>0.011714280995660964</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28" t="s">
         <v>43</v>
       </c>
       <c r="C28" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D28" t="n">
-        <v>0.010236425248376979</v>
+        <v>0.013527098443184227</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B29" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C29" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D29" t="n">
-        <v>0.011779392751982365</v>
+        <v>0.015476120857530695</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C30" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D30" t="n">
-        <v>0.01344345023338589</v>
+        <v>0.017542360183192884</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B31" t="s">
         <v>47</v>
       </c>
       <c r="C31" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D31" t="n">
-        <v>0.015216397462191611</v>
+        <v>0.019700732972561807</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B32" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C32" t="s">
         <v>11</v>
       </c>
       <c r="D32" t="n">
-        <v>0.017081507762573278</v>
+        <v>0.021920234466040966</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B33" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C33" t="s">
         <v>11</v>
       </c>
       <c r="D33" t="n">
-        <v>0.019017517326842093</v>
+        <v>0.02416442447891065</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B34" t="s">
         <v>51</v>
       </c>
       <c r="C34" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D34" t="n">
-        <v>0.02099881067047582</v>
+        <v>0.026392234869326625</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B35" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C35" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D35" t="n">
-        <v>0.022995816511991785</v>
+        <v>0.028559087662930138</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B36" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C36" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D36" t="n">
-        <v>0.0249756173033715</v>
+        <v>0.03061829073868061</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B37" t="s">
         <v>55</v>
       </c>
       <c r="C37" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D37" t="n">
-        <v>0.02690276311076656</v>
+        <v>0.032522656101615754</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B38" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C38" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D38" t="n">
-        <v>0.02874026736006957</v>
+        <v>0.034226266096593155</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C39" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D39" t="n">
-        <v>0.03045074906680717</v>
+        <v>0.035686297332261474</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B40" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C40" t="s">
         <v>6</v>
       </c>
       <c r="D40" t="n">
-        <v>0.0319976745789137</v>
+        <v>0.036864802230996724</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B41" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C41" t="s">
         <v>6</v>
       </c>
       <c r="D41" t="n">
-        <v>0.03334664256440545</v>
+        <v>0.03773034521835793</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B42" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
       </c>
       <c r="D42" t="n">
-        <v>0.03446664984599705</v>
+        <v>0.0382593952557892</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B43" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C43" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D43" t="n">
-        <v>0.03533127338625605</v>
+        <v>0.03843738866572659</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B44" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C44" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D44" t="n">
-        <v>0.03591970564306976</v>
+        <v>0.03825939525578885</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B45" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C45" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D45" t="n">
-        <v>0.03621758669689436</v>
+        <v>0.03773034521835811</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B46" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C46" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D46" t="n">
-        <v>0.03621758669689436</v>
+        <v>0.03686480223099682</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B47" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C47" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D47" t="n">
-        <v>0.03591970564306976</v>
+        <v>0.03568629733226136</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B48" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C48" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D48" t="n">
-        <v>0.03533127338625605</v>
+        <v>0.0342262660965931</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B49" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C49" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D49" t="n">
-        <v>0.03446664984599705</v>
+        <v>0.03252265610161595</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B50" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C50" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D50" t="n">
-        <v>0.03334664256440559</v>
+        <v>0.030618290738680443</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B51" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C51" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D51" t="n">
-        <v>0.0319976745789137</v>
+        <v>0.02855908766293025</v>
       </c>
     </row>
     <row r="52">
@@ -1153,13 +1141,13 @@
         <v>74</v>
       </c>
       <c r="B52" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C52" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D52" t="n">
-        <v>0.03045074906680717</v>
+        <v>0.026392234869326403</v>
       </c>
     </row>
     <row r="53">
@@ -1167,27 +1155,27 @@
         <v>74</v>
       </c>
       <c r="B53" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C53" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D53" t="n">
-        <v>0.028740267360069627</v>
+        <v>0.024164424478910818</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B54" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C54" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D54" t="n">
-        <v>0.026902763110766503</v>
+        <v>0.021920234466040966</v>
       </c>
     </row>
     <row r="55">
@@ -1195,405 +1183,405 @@
         <v>78</v>
       </c>
       <c r="B55" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C55" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D55" t="n">
-        <v>0.02497561730337139</v>
+        <v>0.01970073297256164</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B56" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C56" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D56" t="n">
-        <v>0.022995816511991785</v>
+        <v>0.01754236018319294</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B57" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C57" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D57" t="n">
-        <v>0.02099881067047582</v>
+        <v>0.01547612085753075</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B58" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C58" t="s">
         <v>6</v>
       </c>
       <c r="D58" t="n">
-        <v>0.019017517326842093</v>
+        <v>0.013527098443184116</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B59" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C59" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D59" t="n">
-        <v>0.017081507762573278</v>
+        <v>0.011714280995660964</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B60" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C60" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D60" t="n">
-        <v>0.015216397462191611</v>
+        <v>0.010050671362960117</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B61" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C61" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D61" t="n">
-        <v>0.013443450233386056</v>
+        <v>0.008543640303900951</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B62" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C62" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D62" t="n">
-        <v>0.011779392751982198</v>
+        <v>0.007195471982361333</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B63" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C63" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D63" t="n">
-        <v>0.010236425248376979</v>
+        <v>0.006004046735196614</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B64" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C64" t="s">
         <v>6</v>
       </c>
       <c r="D64" t="n">
-        <v>0.00882240507667209</v>
+        <v>0.004963605855329449</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B65" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C65" t="s">
         <v>6</v>
       </c>
       <c r="D65" t="n">
-        <v>0.007541173401749167</v>
+        <v>0.004065546738784509</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B66" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C66" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D66" t="n">
-        <v>0.0063929913562243805</v>
+        <v>0.0032992032661826754</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B67" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C67" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D67" t="n">
-        <v>0.005375050692804178</v>
+        <v>0.002652574764543508</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B68" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C68" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D68" t="n">
-        <v>0.00448202493663857</v>
+        <v>0.002112976358024406</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B69" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C69" t="s">
         <v>11</v>
       </c>
       <c r="D69" t="n">
-        <v>0.0037066299353480936</v>
+        <v>0.0016675930842951162</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B70" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C70" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D70" t="n">
-        <v>0.003040167032311589</v>
+        <v>0.0013039290942738306</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B71" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C71" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D71" t="n">
-        <v>0.0024730273370353866</v>
+        <v>0.0010101510233837515</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B72" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C72" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D72" t="n">
-        <v>0.001995141233155761</v>
+        <v>7.753308807374672E-4</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B73" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C73" t="s">
         <v>6</v>
       </c>
       <c r="D73" t="n">
-        <v>0.0015963628996320403</v>
+        <v>5.895983997792342E-4</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B74" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C74" t="s">
         <v>6</v>
       </c>
       <c r="D74" t="n">
-        <v>0.0012667848535509027</v>
+        <v>4.4421574738256965E-4</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B75" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C75" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D75" t="n">
-        <v>9.969820791533015E-4</v>
+        <v>3.315889451143343E-4</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B76" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C76" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D76" t="n">
-        <v>7.781890133835537E-4</v>
+        <v>2.452305511357472E-4</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B77" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C77" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D77" t="n">
-        <v>6.024154353669231E-4</v>
+        <v>1.7968736598590222E-4</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B78" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C78" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D78" t="n">
-        <v>4.625091609729505E-4</v>
+        <v>1.3044545353947104E-4</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B79" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C79" t="s">
         <v>11</v>
       </c>
       <c r="D79" t="n">
-        <v>3.5217444534218524E-4</v>
+        <v>9.382288586223236E-5</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B80" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C80" t="s">
         <v>11</v>
       </c>
       <c r="D80" t="n">
-        <v>2.659552638953174E-4</v>
+        <v>6.68585666331496E-5</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>30</v>
+        <v>112</v>
       </c>
       <c r="B81" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C81" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D81" t="n">
-        <v>1.991923211064297E-4</v>
+        <v>4.7203453057844376E-5</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>30</v>
+        <v>116</v>
       </c>
       <c r="B82" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C82" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D82" t="n">
-        <v>1.4796188113642457E-4</v>
+        <v>3.301861938558857E-5</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>30</v>
+        <v>116</v>
       </c>
       <c r="B83" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C83" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D83" t="n">
-        <v>1.0900347552508766E-4</v>
+        <v>2.288297478250206E-5</v>
       </c>
     </row>
     <row r="84">
@@ -1601,83 +1589,13 @@
         <v>116</v>
       </c>
       <c r="B84" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C84" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="D84" t="n">
-        <v>7.964235537476634E-5</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="s">
-        <v>116</v>
-      </c>
-      <c r="B85" t="s">
-        <v>118</v>
-      </c>
-      <c r="C85" t="s">
-        <v>6</v>
-      </c>
-      <c r="D85" t="n">
-        <v>5.7711331430826716E-5</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="s">
-        <v>116</v>
-      </c>
-      <c r="B86" t="s">
-        <v>119</v>
-      </c>
-      <c r="C86" t="s">
-        <v>6</v>
-      </c>
-      <c r="D86" t="n">
-        <v>4.1475472243049575E-5</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="s">
-        <v>120</v>
-      </c>
-      <c r="B87" t="s">
-        <v>121</v>
-      </c>
-      <c r="C87" t="s">
-        <v>6</v>
-      </c>
-      <c r="D87" t="n">
-        <v>2.9562069406283386E-5</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="s">
-        <v>120</v>
-      </c>
-      <c r="B88" t="s">
-        <v>122</v>
-      </c>
-      <c r="C88" t="s">
-        <v>6</v>
-      </c>
-      <c r="D88" t="n">
-        <v>2.089736706111163E-5</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="s">
-        <v>120</v>
-      </c>
-      <c r="B89" t="s">
-        <v>123</v>
-      </c>
-      <c r="C89" t="s">
-        <v>6</v>
-      </c>
-      <c r="D89" t="n">
-        <v>1.4650807275492836E-5</v>
+        <v>1.5712109037655242E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented student integration testing bugged
</commit_message>
<xml_diff>
--- a/src/main/resources/projects60.xlsx
+++ b/src/main/resources/projects60.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="119">
   <si>
     <t>Supervisor</t>
   </si>
@@ -26,361 +26,349 @@
     <t>Probability</t>
   </si>
   <si>
-    <t>Savonarola</t>
-  </si>
-  <si>
-    <t>Florence and the Cthulu mythos</t>
+    <t>Thomas Edison</t>
+  </si>
+  <si>
+    <t>Physics and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>CS+DS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Electricity and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>pioneering new technologies in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Victor Meldrew</t>
+  </si>
+  <si>
+    <t>Modern Britain and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t>complaining about everything in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Malcolm X</t>
+  </si>
+  <si>
+    <t>American politics and the Cthulu mythos</t>
   </si>
   <si>
     <t>CS</t>
   </si>
   <si>
-    <t xml:space="preserve"> the Renaissance and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>promoting conservative values in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Gordon Ramsay</t>
-  </si>
-  <si>
-    <t>Cooking and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Kitchen and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Haute Cuisine and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>Billie Holiday</t>
-  </si>
-  <si>
-    <t>Jazz and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Blues music and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>singing jazz songs in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>David Letterman</t>
-  </si>
-  <si>
-    <t>Late-night TV and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>CS+DS</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Chat Shows and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CBS and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>Stephen Jay Gould</t>
-  </si>
-  <si>
-    <t>Evolution and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Humanism and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>collecting fossils in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Robin Williams</t>
-  </si>
-  <si>
-    <t>Comedy and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hollywood and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Stand-Up Comedy and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>Kim Kardashian</t>
-  </si>
-  <si>
-    <t>Reality TV and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>starring in reality TV shows in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> flaunting buttocks in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Selena Gomez</t>
-  </si>
-  <si>
-    <t>Pop Music and the Cthulu mythos</t>
+    <t xml:space="preserve"> Race Relations and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Black liberation and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>Fagin</t>
+  </si>
+  <si>
+    <t>Oliver Twist and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Victorian literature and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dickensian fiction and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>Conan the Barbarian</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mythology and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Marvel Comics and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Hyborian Age and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>Sam Spade</t>
+  </si>
+  <si>
+    <t>Detective fiction and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>solving mysteries in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> solving crimes in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Annie Oakley</t>
+  </si>
+  <si>
+    <t>American history and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>promoting circus attractions in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> selling tickets in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Marlon Brando</t>
+  </si>
+  <si>
+    <t>Hollywood and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Acting and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>starring in Hollywood movies in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Judy Garland</t>
+  </si>
+  <si>
+    <t>Music and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Musicals and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>singing torch songs in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>George Washington</t>
+  </si>
+  <si>
+    <t>the American War of Independence and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>leading revolutions in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fighting for liberty in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Bernard Madoff</t>
+  </si>
+  <si>
+    <t>Investment Funds and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Investments and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Finance and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>Sheldon Cooper</t>
+  </si>
+  <si>
+    <t>The Big Bang Theory and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>studying science in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> collecting comic books in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Yoda</t>
+  </si>
+  <si>
+    <t>Star Wars and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>fighting for the resistance in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> promoting mysticism in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Han Solo</t>
+  </si>
+  <si>
+    <t>piloting the Millenium Falcon in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> doing the Kessel run in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> smuggling contraband in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Borat</t>
+  </si>
+  <si>
+    <t>Borat! and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Comedy and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Documentaries and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>Joe Louis</t>
+  </si>
+  <si>
+    <t>Boxing and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>winning heavyweight titles in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> knocking out opponents in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Frank Columbo</t>
+  </si>
+  <si>
+    <t>solving crimes in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pursuing criminals in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> tricking criminals in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Ross Geller</t>
+  </si>
+  <si>
+    <t>Friends and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>studying paleontology in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> studying dinosaurs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Barney Rubble</t>
+  </si>
+  <si>
+    <t>Bedrock and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Neolithic times and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>pedalling engine-less cars in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Ringo Starr</t>
+  </si>
+  <si>
+    <t>The Beatles and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pop music and the Cthulu mythos</t>
   </si>
   <si>
     <t>singing pop songs in Cthulhu-worshipping societies</t>
   </si>
   <si>
-    <t xml:space="preserve"> writing pop songs in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Lucille Ball</t>
-  </si>
-  <si>
-    <t>Comedy and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>starring in sit-coms in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> starring in madcap comedies in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Buzz Aldrin</t>
-  </si>
-  <si>
-    <t>NASA and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Space flight and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Moon and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>Kurt Vonnegut</t>
-  </si>
-  <si>
-    <t>American literature and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Dystopian fiction and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>writing science fiction in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Ron Burgundy</t>
-  </si>
-  <si>
-    <t>Anchorman and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>DS</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the News and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>reading the news in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Chuck Norris</t>
-  </si>
-  <si>
-    <t>Hollywood and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Acting and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Action movies and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>Jerry Seinfeld</t>
-  </si>
-  <si>
-    <t>The Seinfeld Chronicles and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Comedy and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>doing stand-up in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Cristiano Ronaldo</t>
-  </si>
-  <si>
-    <t>Soccer and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>playing soccer in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Thomas Edison</t>
-  </si>
-  <si>
-    <t>Physics and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Electricity and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>pioneering new technologies in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>John Wilkes Booth</t>
-  </si>
-  <si>
-    <t>American politics and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>assassinating presidents in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Bruce Willis</t>
-  </si>
-  <si>
-    <t>Hollywood and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Acting and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Action movies and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>Princess Diana</t>
-  </si>
-  <si>
-    <t>Politics and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> British royalty and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> British history and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>Neville Chamberlain</t>
-  </si>
-  <si>
-    <t>World War II and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>appeasing belligerent dictators in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Eleanor Roosevelt</t>
-  </si>
-  <si>
-    <t>American history and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> American politics and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>campaigning for social causes in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Fox Mulder</t>
-  </si>
-  <si>
-    <t>The X-Files and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>postulating bizarre theories in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> investigating alien abductions in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Mister Magoo</t>
-  </si>
-  <si>
-    <t>Comedy and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Animation and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>causing mayhem in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Hillary Clinton</t>
-  </si>
-  <si>
-    <t>American politics and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Left and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Democrats and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>Rush Limbaugh</t>
-  </si>
-  <si>
-    <t>the Right and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Republicans and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Fox News and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>Silvio Berlusconi</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> European politics and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Italy and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>throwing Bunga Bunga parties in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Gwyneth Paltrow</t>
-  </si>
-  <si>
-    <t>running a new-age website in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> starring in Hollywood movies in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> raising new-age children in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Antonio Vivaldi</t>
-  </si>
-  <si>
-    <t>Classical music and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>composing classical music in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>David Blaine</t>
-  </si>
-  <si>
-    <t>Magic and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Street Magic and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>performing street magic in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Tony Montana</t>
-  </si>
-  <si>
-    <t>the Miami crime world and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>running a crime family in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> running an empire in Dagon-worshipping societies</t>
+    <t>Johann von Goethe</t>
+  </si>
+  <si>
+    <t>German literature and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Romantic poetry and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>writing poetry in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Hercule Poirot</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Drawing room mysteries and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>Jamie Oliver</t>
+  </si>
+  <si>
+    <t>Cooking and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Kitchen and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>cooking dinners in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Don Draper</t>
+  </si>
+  <si>
+    <t>Mad Men and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Advertising Industry and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>developing advertising campaigns in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Robert De Niro</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Serious Acting and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>Dr. Julius No</t>
+  </si>
+  <si>
+    <t>James Bond and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Terrorism and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Finance and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>Michelangelo</t>
+  </si>
+  <si>
+    <t>Renaissance art and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sculpture and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Painting and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>Cleopatra</t>
+  </si>
+  <si>
+    <t>Ancient Egypt and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>seducing emperors in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Dante Alighieri</t>
+  </si>
+  <si>
+    <t>Italian literature and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Italian poetry and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>Johnny Cash</t>
+  </si>
+  <si>
+    <t>Country music and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>singing country music in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
   </si>
 </sst>
 </file>
@@ -456,7 +444,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="n">
-        <v>1.505783055364567E-5</v>
+        <v>1.5942874282766786E-5</v>
       </c>
     </row>
     <row r="3">
@@ -470,7 +458,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="n">
-        <v>2.1651536583204518E-5</v>
+        <v>2.332292012013505E-5</v>
       </c>
     </row>
     <row r="4">
@@ -484,7 +472,7 @@
         <v>6</v>
       </c>
       <c r="D4" t="n">
-        <v>3.086452805560744E-5</v>
+        <v>3.3796272679214874E-5</v>
       </c>
     </row>
     <row r="5">
@@ -495,10 +483,10 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D5" t="n">
-        <v>4.3618945181192063E-5</v>
+        <v>4.850921699096642E-5</v>
       </c>
     </row>
     <row r="6">
@@ -506,27 +494,27 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D6" t="n">
-        <v>6.111323578402071E-5</v>
+        <v>6.896826537182673E-5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D7" t="n">
-        <v>8.488676861496594E-5</v>
+        <v>9.712788286860436E-5</v>
       </c>
     </row>
     <row r="8">
@@ -534,13 +522,13 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D8" t="n">
-        <v>1.1689322142142652E-4</v>
+        <v>1.3549027469737871E-4</v>
       </c>
     </row>
     <row r="9">
@@ -548,69 +536,69 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D9" t="n">
-        <v>1.595817624250387E-4</v>
+        <v>1.872155451685322E-4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D10" t="n">
-        <v>2.1598410522086274E-4</v>
+        <v>2.562390256479521E-4</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D11" t="n">
-        <v>2.898043709736888E-4</v>
+        <v>3.473907308082161E-4</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D12" t="n">
-        <v>3.855073630913083E-4</v>
+        <v>4.6650979195683165E-4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D13" t="n">
-        <v>5.083994008726104E-4</v>
+        <v>6.205444391459215E-4</v>
       </c>
     </row>
     <row r="14">
@@ -618,13 +606,13 @@
         <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D14" t="n">
-        <v>6.646943545436847E-4</v>
+        <v>8.176258239262317E-4</v>
       </c>
     </row>
     <row r="15">
@@ -632,27 +620,27 @@
         <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D15" t="n">
-        <v>8.615560933513725E-4</v>
+        <v>0.0010671019160250375</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D16" t="n">
-        <v>0.001107107352715952</v>
+        <v>0.0013795161487181315</v>
       </c>
     </row>
     <row r="17">
@@ -660,13 +648,13 @@
         <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0014103942251250208</v>
+        <v>0.0017665147484438194</v>
       </c>
     </row>
     <row r="18">
@@ -674,27 +662,27 @@
         <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0017812952787859193</v>
+        <v>0.002240667099338698</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0022303649055994993</v>
+        <v>0.0028151853791836615</v>
       </c>
     </row>
     <row r="20">
@@ -702,13 +690,13 @@
         <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D20" t="n">
-        <v>0.002768602073801108</v>
+        <v>0.003503533314246604</v>
       </c>
     </row>
     <row r="21">
@@ -716,27 +704,27 @@
         <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D21" t="n">
-        <v>0.003407138344583718</v>
+        <v>0.004318919381253825</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D22" t="n">
-        <v>0.004156842869608986</v>
+        <v>0.005273677121735702</v>
       </c>
     </row>
     <row r="23">
@@ -744,13 +732,13 @@
         <v>34</v>
       </c>
       <c r="B23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D23" t="n">
-        <v>0.0050278470850103375</v>
+        <v>0.0063785442143808775</v>
       </c>
     </row>
     <row r="24">
@@ -758,27 +746,27 @@
         <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D24" t="n">
-        <v>0.006028997807761845</v>
+        <v>0.007641862135260906</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
         <v>6</v>
       </c>
       <c r="D25" t="n">
-        <v>0.007167254142553786</v>
+        <v>0.009068728952038141</v>
       </c>
     </row>
     <row r="26">
@@ -786,13 +774,13 @@
         <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D26" t="n">
-        <v>0.008447050610743002</v>
+        <v>0.010660148164411132</v>
       </c>
     </row>
     <row r="27">
@@ -800,27 +788,27 @@
         <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C27" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D27" t="n">
-        <v>0.009869655688586887</v>
+        <v>0.01241222547987647</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C28" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D28" t="n">
-        <v>0.011432560872336073</v>
+        <v>0.014315471889394582</v>
       </c>
     </row>
     <row r="29">
@@ -828,13 +816,13 @@
         <v>42</v>
       </c>
       <c r="B29" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C29" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D29" t="n">
-        <v>0.013128939812225127</v>
+        <v>0.016354274307613326</v>
       </c>
     </row>
     <row r="30">
@@ -842,27 +830,27 @@
         <v>42</v>
       </c>
       <c r="B30" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C30" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D30" t="n">
-        <v>0.014947219331531203</v>
+        <v>0.01850659345860939</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B31" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C31" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D31" t="n">
-        <v>0.016870803711083293</v>
+        <v>0.02074394200911256</v>
       </c>
     </row>
     <row r="32">
@@ -870,13 +858,13 @@
         <v>46</v>
       </c>
       <c r="B32" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
       </c>
       <c r="D32" t="n">
-        <v>0.018877990070226114</v>
+        <v>0.02303168398030503</v>
       </c>
     </row>
     <row r="33">
@@ -884,27 +872,27 @@
         <v>46</v>
       </c>
       <c r="B33" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C33" t="s">
         <v>6</v>
       </c>
       <c r="D33" t="n">
-        <v>0.020942105831001756</v>
+        <v>0.025329679511732095</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B34" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C34" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D34" t="n">
-        <v>0.023031889205752942</v>
+        <v>0.027593277953685713</v>
       </c>
     </row>
     <row r="35">
@@ -912,13 +900,13 @@
         <v>50</v>
       </c>
       <c r="B35" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C35" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="D35" t="n">
-        <v>0.025112120796158655</v>
+        <v>0.02977463839715333</v>
       </c>
     </row>
     <row r="36">
@@ -929,136 +917,136 @@
         <v>53</v>
       </c>
       <c r="C36" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="D36" t="n">
-        <v>0.02714449943490027</v>
+        <v>0.03182433192119388</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B37" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C37" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="D37" t="n">
-        <v>0.029088739313355316</v>
+        <v>0.033693156147072634</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B38" t="s">
         <v>56</v>
       </c>
       <c r="C38" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D38" t="n">
-        <v>0.030903849400578998</v>
+        <v>0.035334072333491895</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B39" t="s">
         <v>57</v>
       </c>
       <c r="C39" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D39" t="n">
-        <v>0.03254954146350572</v>
+        <v>0.03670416029370041</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B40" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C40" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D40" t="n">
-        <v>0.03398770093550979</v>
+        <v>0.037766478566174294</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B41" t="s">
         <v>60</v>
       </c>
       <c r="C41" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D41" t="n">
-        <v>0.03518384661026934</v>
+        <v>0.03849171765824959</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B42" t="s">
         <v>61</v>
       </c>
       <c r="C42" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D42" t="n">
-        <v>0.036108501568554774</v>
+        <v>0.03885954321210054</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B43" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C43" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D43" t="n">
-        <v>0.03673839942888419</v>
+        <v>0.03885954321210054</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B44" t="s">
         <v>64</v>
       </c>
       <c r="C44" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D44" t="n">
-        <v>0.0370574570707446</v>
+        <v>0.03849171765824978</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B45" t="s">
         <v>65</v>
       </c>
       <c r="C45" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D45" t="n">
-        <v>0.0370574570707446</v>
+        <v>0.037766478566174266</v>
       </c>
     </row>
     <row r="46">
@@ -1069,10 +1057,10 @@
         <v>67</v>
       </c>
       <c r="C46" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D46" t="n">
-        <v>0.036738399428884315</v>
+        <v>0.03670416029370038</v>
       </c>
     </row>
     <row r="47">
@@ -1083,10 +1071,10 @@
         <v>68</v>
       </c>
       <c r="C47" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D47" t="n">
-        <v>0.036108501568554566</v>
+        <v>0.03533407233349195</v>
       </c>
     </row>
     <row r="48">
@@ -1097,10 +1085,10 @@
         <v>69</v>
       </c>
       <c r="C48" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D48" t="n">
-        <v>0.035183846610269284</v>
+        <v>0.03369315614707258</v>
       </c>
     </row>
     <row r="49">
@@ -1111,10 +1099,10 @@
         <v>71</v>
       </c>
       <c r="C49" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D49" t="n">
-        <v>0.03398770093550993</v>
+        <v>0.03182433192119405</v>
       </c>
     </row>
     <row r="50">
@@ -1125,155 +1113,155 @@
         <v>72</v>
       </c>
       <c r="C50" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D50" t="n">
-        <v>0.03254954146350572</v>
+        <v>0.029774638397153053</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
+        <v>70</v>
+      </c>
+      <c r="B51" t="s">
         <v>73</v>
       </c>
-      <c r="B51" t="s">
-        <v>74</v>
-      </c>
       <c r="C51" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D51" t="n">
-        <v>0.030903849400578998</v>
+        <v>0.027593277953685713</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B52" t="s">
         <v>75</v>
       </c>
       <c r="C52" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D52" t="n">
-        <v>0.029088739313355205</v>
+        <v>0.025329679511732095</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B53" t="s">
         <v>76</v>
       </c>
       <c r="C53" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D53" t="n">
-        <v>0.02714449943490016</v>
+        <v>0.02303168398030503</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
+        <v>74</v>
+      </c>
+      <c r="B54" t="s">
         <v>77</v>
       </c>
-      <c r="B54" t="s">
-        <v>78</v>
-      </c>
       <c r="C54" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D54" t="n">
-        <v>0.025112120796158877</v>
+        <v>0.020743942009112726</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B55" t="s">
         <v>79</v>
       </c>
       <c r="C55" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D55" t="n">
-        <v>0.023031889205752942</v>
+        <v>0.018506593458609277</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B56" t="s">
         <v>80</v>
       </c>
       <c r="C56" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D56" t="n">
-        <v>0.020942105831001756</v>
+        <v>0.016354274307613437</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
+        <v>78</v>
+      </c>
+      <c r="B57" t="s">
         <v>81</v>
       </c>
-      <c r="B57" t="s">
-        <v>82</v>
-      </c>
       <c r="C57" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D57" t="n">
-        <v>0.018877990070226225</v>
+        <v>0.014315471889394471</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B58" t="s">
         <v>83</v>
       </c>
       <c r="C58" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D58" t="n">
-        <v>0.016870803711083127</v>
+        <v>0.01241222547987647</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
+        <v>82</v>
+      </c>
+      <c r="B59" t="s">
         <v>84</v>
       </c>
-      <c r="B59" t="s">
-        <v>85</v>
-      </c>
       <c r="C59" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D59" t="n">
-        <v>0.014947219331531258</v>
+        <v>0.010660148164411076</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B60" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C60" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D60" t="n">
-        <v>0.013128939812225127</v>
+        <v>0.009068728952038141</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B61" t="s">
         <v>87</v>
@@ -1282,49 +1270,49 @@
         <v>6</v>
       </c>
       <c r="D61" t="n">
-        <v>0.011432560872336073</v>
+        <v>0.007641862135260906</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
+        <v>86</v>
+      </c>
+      <c r="B62" t="s">
         <v>88</v>
       </c>
-      <c r="B62" t="s">
-        <v>89</v>
-      </c>
       <c r="C62" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D62" t="n">
-        <v>0.009869655688586942</v>
+        <v>0.0063785442143808775</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B63" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C63" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D63" t="n">
-        <v>0.008447050610742905</v>
+        <v>0.005273677121735702</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B64" t="s">
         <v>91</v>
       </c>
       <c r="C64" t="s">
-        <v>52</v>
+        <v>11</v>
       </c>
       <c r="D64" t="n">
-        <v>0.0071672541425537376</v>
+        <v>0.004318919381253825</v>
       </c>
     </row>
     <row r="65">
@@ -1335,10 +1323,10 @@
         <v>93</v>
       </c>
       <c r="C65" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D65" t="n">
-        <v>0.006028997807761935</v>
+        <v>0.003503533314246604</v>
       </c>
     </row>
     <row r="66">
@@ -1349,10 +1337,10 @@
         <v>94</v>
       </c>
       <c r="C66" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D66" t="n">
-        <v>0.0050278470850103375</v>
+        <v>0.0028151853791836823</v>
       </c>
     </row>
     <row r="67">
@@ -1363,10 +1351,10 @@
         <v>95</v>
       </c>
       <c r="C67" t="s">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="D67" t="n">
-        <v>0.004156842869608986</v>
+        <v>0.002240667099338677</v>
       </c>
     </row>
     <row r="68">
@@ -1377,10 +1365,10 @@
         <v>97</v>
       </c>
       <c r="C68" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D68" t="n">
-        <v>0.003407138344583697</v>
+        <v>0.001766514748443821</v>
       </c>
     </row>
     <row r="69">
@@ -1391,10 +1379,10 @@
         <v>98</v>
       </c>
       <c r="C69" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D69" t="n">
-        <v>0.0027686020738011026</v>
+        <v>0.0013795161487181358</v>
       </c>
     </row>
     <row r="70">
@@ -1405,10 +1393,10 @@
         <v>99</v>
       </c>
       <c r="C70" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D70" t="n">
-        <v>0.0022303649055995254</v>
+        <v>0.0010671019160250375</v>
       </c>
     </row>
     <row r="71">
@@ -1419,234 +1407,178 @@
         <v>101</v>
       </c>
       <c r="C71" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D71" t="n">
-        <v>0.0017812952787859193</v>
+        <v>8.176258239262256E-4</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B72" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C72" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D72" t="n">
-        <v>0.0014103942251250208</v>
+        <v>6.205444391459215E-4</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B73" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C73" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D73" t="n">
-        <v>0.0011071073527159432</v>
+        <v>4.6650979195683165E-4</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B74" t="s">
         <v>105</v>
       </c>
       <c r="C74" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D74" t="n">
-        <v>8.615560933513768E-4</v>
+        <v>3.473907308082161E-4</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B75" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C75" t="s">
         <v>6</v>
       </c>
       <c r="D75" t="n">
-        <v>6.646943545436891E-4</v>
+        <v>2.562390256479521E-4</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B76" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C76" t="s">
         <v>6</v>
       </c>
       <c r="D76" t="n">
-        <v>5.083994008726104E-4</v>
+        <v>1.8721554516853403E-4</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B77" t="s">
         <v>109</v>
       </c>
       <c r="C77" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="D77" t="n">
-        <v>3.855073630913083E-4</v>
+        <v>1.3549027469737774E-4</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B78" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C78" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D78" t="n">
-        <v>2.898043709736888E-4</v>
+        <v>9.712788286860396E-5</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B79" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C79" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D79" t="n">
-        <v>2.1598410522086155E-4</v>
+        <v>6.89682653718266E-5</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B80" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C80" t="s">
         <v>6</v>
       </c>
       <c r="D80" t="n">
-        <v>1.5958176242503988E-4</v>
+        <v>4.85092169909665E-5</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B81" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C81" t="s">
         <v>6</v>
       </c>
       <c r="D81" t="n">
-        <v>1.1689322142142652E-4</v>
+        <v>3.379627267921447E-5</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B82" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C82" t="s">
         <v>6</v>
       </c>
       <c r="D82" t="n">
-        <v>8.488676861496594E-5</v>
+        <v>2.332292012013505E-5</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B83" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C83" t="s">
         <v>6</v>
       </c>
       <c r="D83" t="n">
-        <v>6.111323578402071E-5</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="s">
-        <v>115</v>
-      </c>
-      <c r="B84" t="s">
-        <v>118</v>
-      </c>
-      <c r="C84" t="s">
-        <v>6</v>
-      </c>
-      <c r="D84" t="n">
-        <v>4.361894518119189E-5</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="s">
-        <v>119</v>
-      </c>
-      <c r="B85" t="s">
-        <v>120</v>
-      </c>
-      <c r="C85" t="s">
-        <v>52</v>
-      </c>
-      <c r="D85" t="n">
-        <v>3.08645280556074E-5</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="s">
-        <v>119</v>
-      </c>
-      <c r="B86" t="s">
-        <v>121</v>
-      </c>
-      <c r="C86" t="s">
-        <v>52</v>
-      </c>
-      <c r="D86" t="n">
-        <v>2.1651536583204735E-5</v>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="s">
-        <v>119</v>
-      </c>
-      <c r="B87" t="s">
-        <v>122</v>
-      </c>
-      <c r="C87" t="s">
-        <v>52</v>
-      </c>
-      <c r="D87" t="n">
-        <v>1.505783055364567E-5</v>
+        <v>1.5942874282766786E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
algorithm implemented but not tested
</commit_message>
<xml_diff>
--- a/src/main/resources/projects60.xlsx
+++ b/src/main/resources/projects60.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="124">
   <si>
     <t>Supervisor</t>
   </si>
@@ -26,31 +26,355 @@
     <t>Probability</t>
   </si>
   <si>
-    <t>Robert Downey Jr.</t>
+    <t>Diana Ross</t>
+  </si>
+  <si>
+    <t>Pop music and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>CS+DS</t>
+  </si>
+  <si>
+    <t>singing pop songs in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> writing pop songs in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Brian Wilson</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Love songs and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Beach Boys and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>waxing a surfboard in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Niles Crane</t>
+  </si>
+  <si>
+    <t>Psychiatry and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Psychoanalysis and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>nurturing sibling rivalry in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Coriolanus Snow</t>
+  </si>
+  <si>
+    <t>Science Fiction and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Hunger Games and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>running a bureaucracy in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Michelle Obama</t>
+  </si>
+  <si>
+    <t>the Left and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Democrats and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> American politics and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>Scarlett Johansson</t>
   </si>
   <si>
     <t>Hollywood and the Cthulu-Dagon mythos</t>
   </si>
   <si>
-    <t>CS+DS</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Acting and the Cthulu-Dagon mythos</t>
   </si>
   <si>
-    <t xml:space="preserve"> Action movies and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>Captain William Bligh</t>
-  </si>
-  <si>
-    <t>Mutiny on the Bounty and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Politics and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> British history and the Cthulu-Dagon mythos</t>
+    <t>cross-dressing in women's clothes in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Naomi Campbell</t>
+  </si>
+  <si>
+    <t>Fashion and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Rag Trade and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Fashion industry and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>Monica Geller</t>
+  </si>
+  <si>
+    <t>Friends and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>arranging dinner parties in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cooking for friends in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Hercule Poirot</t>
+  </si>
+  <si>
+    <t>Detective fiction and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Drawing room mysteries and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>solving crimes in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Katy Perry</t>
+  </si>
+  <si>
+    <t>Pop Music and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>singing pop songs in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> writing pop songs in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Marcel Duchamp</t>
+  </si>
+  <si>
+    <t>Dadaism and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Modern art and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>making subversive art in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Ernst Stavro Blofeld</t>
+  </si>
+  <si>
+    <t>James Bond and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Terrorism and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Finance and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>James T. Kirk</t>
+  </si>
+  <si>
+    <t>Star Trek and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the U.S.S. Enterprise and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Starfleet and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>Peter Parker</t>
+  </si>
+  <si>
+    <t>Marvel Comics and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>studying science in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> maintaining a secret identity in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Galileo Galilei</t>
+  </si>
+  <si>
+    <t>Physics and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Astronomy and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Cosmos and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>Henry Kissinger</t>
+  </si>
+  <si>
+    <t>the Right and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the Republicans and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>brokering peace deals in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Meghan Markle</t>
+  </si>
+  <si>
+    <t>British royalty and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>racking up marriages in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Andrew Lloyd Webber</t>
+  </si>
+  <si>
+    <t>Musicals and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Musical Theatre and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>making insipid musicals in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Chuck Norris</t>
+  </si>
+  <si>
+    <t>Hollywood and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Acting and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Action movies and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>Jerry Maguire</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> American sports and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> American football and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>promoting greed in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Popeye</t>
+  </si>
+  <si>
+    <t>Thimble Theatre and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>foiling the schemes of evil villains in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> defending the weak in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Bill Gates</t>
+  </si>
+  <si>
+    <t>Microsoft and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Technology and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Software and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>Serena Williams</t>
+  </si>
+  <si>
+    <t>Tennis and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>delivering forehand slams in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> winning tennis tournaments in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Fred Flintstone</t>
+  </si>
+  <si>
+    <t>Bedrock and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Neolithic times and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>pedalling engine-less cars in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Dorothy Parker</t>
+  </si>
+  <si>
+    <t>American literature and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Algonquin Round Table and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>writing for the New Yorker in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Lex Luthor</t>
+  </si>
+  <si>
+    <t>DC Comics and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Metropolis and the Dagon mythos</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Big business and the Dagon mythos</t>
+  </si>
+  <si>
+    <t>Bono</t>
+  </si>
+  <si>
+    <t>Rock music and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>singing rock songs in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> avoiding taxes in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t>Daniel Boone</t>
+  </si>
+  <si>
+    <t>the American West and the Cthulu-Dagon mythos</t>
+  </si>
+  <si>
+    <t>hunting raccoons in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
+  </si>
+  <si>
+    <t>Steven Spielberg</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Special Effects and the Cthulu mythos</t>
+  </si>
+  <si>
+    <t>directing Hollywood movies in Cthulhu-worshipping societies</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> producing Hollywood movies in Cthulhu-worshipping societies</t>
   </si>
   <si>
     <t>Henry James</t>
@@ -60,333 +384,6 @@
   </si>
   <si>
     <t>writing modern fiction in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Eddy Merckx</t>
-  </si>
-  <si>
-    <t>Cycling and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>pedalling furiously in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> winning cycling races in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Christian Grey</t>
-  </si>
-  <si>
-    <t>Fifty Shades of Grey and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>DS</t>
-  </si>
-  <si>
-    <t>running a multinational corporation in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> seducing women in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Sean Hannity</t>
-  </si>
-  <si>
-    <t>the Right and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>CS</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Republicans and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> American politics and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>William the Conqueror</t>
-  </si>
-  <si>
-    <t>British history and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>fighting with swords in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> leading armies into battle in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Russell Brand</t>
-  </si>
-  <si>
-    <t>British comedy and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> British humour and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Comedy and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>Carl Lewis</t>
-  </si>
-  <si>
-    <t>Athletics and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Olympics and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>winning gold medals in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Baldrick</t>
-  </si>
-  <si>
-    <t>the English class system and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>developing cunning plans in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> providing comic relief in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Hedda Hopper</t>
-  </si>
-  <si>
-    <t>Hollywood and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Newspaper industry and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>promoting conservative values in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>James T. Kirk</t>
-  </si>
-  <si>
-    <t>Star Trek and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the U.S.S. Enterprise and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Starfleet and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>Jamie Oliver</t>
-  </si>
-  <si>
-    <t>Cooking and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Kitchen and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>cooking dinners in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Pablo Picasso</t>
-  </si>
-  <si>
-    <t>Modern art and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cubism and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>painting abstract pictures in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Katniss Everdeen</t>
-  </si>
-  <si>
-    <t>Science Fiction and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The Hunger Games and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>fighting for justice in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Pyotr Ilyich Tchaikovsky</t>
-  </si>
-  <si>
-    <t>Classical music and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Piano music and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>composing classical music in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Sir Hugo Drax</t>
-  </si>
-  <si>
-    <t>James Bond and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Terrorism and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Finance and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>Dean Winchester</t>
-  </si>
-  <si>
-    <t>Horror and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Supernatural and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Demonology and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>Jabba the Hutt</t>
-  </si>
-  <si>
-    <t>Star Wars and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>running a crime family in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> running a smuggling business in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Norma Desmond</t>
-  </si>
-  <si>
-    <t>Sunset Boulevard and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Hollywood and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>clinging to past dreams in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Genghis Khan</t>
-  </si>
-  <si>
-    <t>the Mongols and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mongolia and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>running an empire in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Atticus Finch</t>
-  </si>
-  <si>
-    <t>the Law and the Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the American South and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>representing the disenfranchised in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Francis Crick</t>
-  </si>
-  <si>
-    <t>Biology and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> DNA and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The Double Helix and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>Tarzan</t>
-  </si>
-  <si>
-    <t>the Jungle and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>swinging from tree to tree in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> communicating with animals in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Christopher Columbus</t>
-  </si>
-  <si>
-    <t>the Americas and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Age of Discovery and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t>searching for a new world in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>John McClane</t>
-  </si>
-  <si>
-    <t>Die Hard and the Dagon mythos</t>
-  </si>
-  <si>
-    <t>foiling the schemes of evil villains in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> rescuing hostages in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>John McCain</t>
-  </si>
-  <si>
-    <t>running for the senate in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> campaigning for the presidency in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> making maverick choices in Cthulhu-worshipping societies</t>
-  </si>
-  <si>
-    <t>Cooking and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Kitchen and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>cooking dinners in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Croesus</t>
-  </si>
-  <si>
-    <t>Lydia and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> the Ancient world and the Cthulu-Dagon mythos</t>
-  </si>
-  <si>
-    <t>collecting treasures in Cthulhu-worshipping societies vs in Dagon-worshipping societies</t>
-  </si>
-  <si>
-    <t>Tim Berners-Lee</t>
-  </si>
-  <si>
-    <t>The World Wide Web and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The Internet and the Cthulu mythos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Computers and the Cthulu mythos</t>
   </si>
 </sst>
 </file>
@@ -462,7 +459,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="n">
-        <v>1.4455357427856575E-5</v>
+        <v>1.4851559397829867E-5</v>
       </c>
     </row>
     <row r="3">
@@ -476,7 +473,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="n">
-        <v>2.053847126341509E-5</v>
+        <v>2.1268196140727013E-5</v>
       </c>
     </row>
     <row r="4">
@@ -490,7 +487,7 @@
         <v>6</v>
       </c>
       <c r="D4" t="n">
-        <v>2.894681165097884E-5</v>
+        <v>3.0200882409903816E-5</v>
       </c>
     </row>
     <row r="5">
@@ -504,7 +501,7 @@
         <v>6</v>
       </c>
       <c r="D5" t="n">
-        <v>4.046939361783236E-5</v>
+        <v>4.252447727799545E-5</v>
       </c>
     </row>
     <row r="6">
@@ -518,7 +515,7 @@
         <v>6</v>
       </c>
       <c r="D6" t="n">
-        <v>5.612366203345721E-5</v>
+        <v>5.9372961519356404E-5</v>
       </c>
     </row>
     <row r="7">
@@ -532,7 +529,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="n">
-        <v>7.720735007968847E-5</v>
+        <v>8.219943220723818E-5</v>
       </c>
     </row>
     <row r="8">
@@ -543,10 +540,10 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D8" t="n">
-        <v>1.053573008583764E-4</v>
+        <v>1.1284421543794224E-4</v>
       </c>
     </row>
     <row r="9">
@@ -554,153 +551,153 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D9" t="n">
-        <v>1.42614593609708E-4</v>
+        <v>1.5361023868065086E-4</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D10" t="n">
-        <v>1.914946502662194E-4</v>
+        <v>2.0734396824795775E-4</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D11" t="n">
-        <v>2.5506018331189527E-4</v>
+        <v>2.77519195718153E-4</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D12" t="n">
-        <v>3.3699389603134456E-4</v>
+        <v>3.683197703472972E-4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
         <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D13" t="n">
-        <v>4.416667927249001E-4</v>
+        <v>4.8471606686904356E-4</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D14" t="n">
-        <v>5.741968515153516E-4</v>
+        <v>6.325286215140115E-4</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
         <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D15" t="n">
-        <v>7.404917306698114E-4</v>
+        <v>8.184710652093482E-4</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
         <v>25</v>
       </c>
-      <c r="B16" t="s">
-        <v>26</v>
-      </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D16" t="n">
-        <v>9.472682180555855E-4</v>
+        <v>0.0010501633623933352</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0012020404095168134</v>
+        <v>0.0013361055821213335</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0015130682470696037</v>
+        <v>0.0016856021568725224</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0018892581989318254</v>
+        <v>0.00210862699870843</v>
       </c>
     </row>
     <row r="20">
@@ -708,13 +705,13 @@
         <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D20" t="n">
-        <v>0.0023400086511542965</v>
+        <v>0.0026156211031990416</v>
       </c>
     </row>
     <row r="21">
@@ -725,365 +722,365 @@
         <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D21" t="n">
-        <v>0.0028749941144059713</v>
+        <v>0.0032172165050838933</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" t="s">
         <v>34</v>
       </c>
-      <c r="B22" t="s">
-        <v>35</v>
-      </c>
       <c r="C22" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="D22" t="n">
-        <v>0.003503884700880403</v>
+        <v>0.003923883724839457</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
         <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D23" t="n">
-        <v>0.004236000512180264</v>
+        <v>0.0047455041513748235</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B24" t="s">
         <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D24" t="n">
-        <v>0.005079904546061047</v>
+        <v>0.005690874033349825</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" t="s">
         <v>38</v>
       </c>
-      <c r="B25" t="s">
-        <v>39</v>
-      </c>
       <c r="C25" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D25" t="n">
-        <v>0.006042942342825555</v>
+        <v>0.006767152678813563</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B26" t="s">
         <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D26" t="n">
-        <v>0.007130741627938725</v>
+        <v>0.007979273753471877</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B27" t="s">
         <v>41</v>
       </c>
       <c r="C27" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D27" t="n">
-        <v>0.008346690357448165</v>
+        <v>0.009329344778666426</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" t="s">
         <v>42</v>
       </c>
-      <c r="B28" t="s">
-        <v>43</v>
-      </c>
       <c r="C28" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D28" t="n">
-        <v>0.009691416454386426</v>
+        <v>0.01081606553293224</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B29" t="s">
         <v>44</v>
       </c>
       <c r="C29" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D29" t="n">
-        <v>0.011162296702602659</v>
+        <v>0.012434200478872948</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B30" t="s">
         <v>45</v>
       </c>
       <c r="C30" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D30" t="n">
-        <v>0.012753025283739616</v>
+        <v>0.014174142992357697</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" t="s">
         <v>46</v>
       </c>
-      <c r="B31" t="s">
-        <v>47</v>
-      </c>
       <c r="C31" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D31" t="n">
-        <v>0.014453273866615934</v>
+        <v>0.01602160954283749</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B32" t="s">
         <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D32" t="n">
-        <v>0.016248474612823693</v>
+        <v>0.017957499659263798</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B33" t="s">
         <v>49</v>
       </c>
       <c r="C33" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D33" t="n">
-        <v>0.018119754684082556</v>
+        <v>0.019957952290163616</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" t="s">
         <v>50</v>
       </c>
-      <c r="B34" t="s">
-        <v>51</v>
-      </c>
       <c r="C34" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D34" t="n">
-        <v>0.020044045712877323</v>
+        <v>0.02199462103004135</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B35" t="s">
         <v>52</v>
       </c>
       <c r="C35" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D35" t="n">
-        <v>0.02199438429916989</v>
+        <v>0.024035179897379078</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B36" t="s">
         <v>53</v>
       </c>
       <c r="C36" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D36" t="n">
-        <v>0.023940410195486705</v>
+        <v>0.026044058440509943</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" t="s">
         <v>54</v>
       </c>
-      <c r="B37" t="s">
-        <v>55</v>
-      </c>
       <c r="C37" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D37" t="n">
-        <v>0.02584905791637604</v>
+        <v>0.02798339069524164</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B38" t="s">
         <v>56</v>
       </c>
       <c r="C38" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D38" t="n">
-        <v>0.027685425714518597</v>
+        <v>0.029814147905219246</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B39" t="s">
         <v>57</v>
       </c>
       <c r="C39" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D39" t="n">
-        <v>0.029413794005321903</v>
+        <v>0.03149741105644363</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" t="s">
         <v>58</v>
       </c>
-      <c r="B40" t="s">
-        <v>59</v>
-      </c>
       <c r="C40" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D40" t="n">
-        <v>0.030998754278076524</v>
+        <v>0.03299572732207945</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B41" t="s">
         <v>60</v>
       </c>
       <c r="C41" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D41" t="n">
-        <v>0.03240640019806401</v>
+        <v>0.03427448554401777</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B42" t="s">
         <v>61</v>
       </c>
       <c r="C42" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D42" t="n">
-        <v>0.03360552580288095</v>
+        <v>0.0353032407972312</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" t="s">
         <v>62</v>
       </c>
-      <c r="B43" t="s">
-        <v>63</v>
-      </c>
       <c r="C43" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D43" t="n">
-        <v>0.0345687720996196</v>
+        <v>0.03605691751988802</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B44" t="s">
         <v>64</v>
       </c>
       <c r="C44" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D44" t="n">
-        <v>0.03527366342805367</v>
+        <v>0.03651682492318803</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B45" t="s">
         <v>65</v>
       </c>
       <c r="C45" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D45" t="n">
-        <v>0.03570347884459607</v>
+        <v>0.03667142730125568</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
+        <v>63</v>
+      </c>
+      <c r="B46" t="s">
         <v>66</v>
       </c>
-      <c r="B46" t="s">
-        <v>67</v>
-      </c>
       <c r="C46" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="D46" t="n">
-        <v>0.035847911374691226</v>
+        <v>0.03651682492318786</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B47" t="s">
         <v>68</v>
@@ -1092,12 +1089,12 @@
         <v>6</v>
       </c>
       <c r="D47" t="n">
-        <v>0.035703478844595724</v>
+        <v>0.03605691751988802</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B48" t="s">
         <v>69</v>
@@ -1106,49 +1103,49 @@
         <v>6</v>
       </c>
       <c r="D48" t="n">
-        <v>0.03527366342805382</v>
+        <v>0.0353032407972312</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
+        <v>67</v>
+      </c>
+      <c r="B49" t="s">
         <v>70</v>
       </c>
-      <c r="B49" t="s">
-        <v>71</v>
-      </c>
       <c r="C49" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D49" t="n">
-        <v>0.03456877209961981</v>
+        <v>0.03427448554401777</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B50" t="s">
         <v>72</v>
       </c>
       <c r="C50" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D50" t="n">
-        <v>0.03360552580288095</v>
+        <v>0.03299572732207945</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B51" t="s">
         <v>73</v>
       </c>
       <c r="C51" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D51" t="n">
-        <v>0.03240640019806401</v>
+        <v>0.031497411056443436</v>
       </c>
     </row>
     <row r="52">
@@ -1159,10 +1156,10 @@
         <v>75</v>
       </c>
       <c r="C52" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D52" t="n">
-        <v>0.030998754278076385</v>
+        <v>0.029814147905219357</v>
       </c>
     </row>
     <row r="53">
@@ -1173,10 +1170,10 @@
         <v>76</v>
       </c>
       <c r="C53" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D53" t="n">
-        <v>0.02941379400532204</v>
+        <v>0.027983390695241472</v>
       </c>
     </row>
     <row r="54">
@@ -1187,10 +1184,10 @@
         <v>77</v>
       </c>
       <c r="C54" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="D54" t="n">
-        <v>0.027685425714518597</v>
+        <v>0.02604405844051022</v>
       </c>
     </row>
     <row r="55">
@@ -1201,10 +1198,10 @@
         <v>79</v>
       </c>
       <c r="C55" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D55" t="n">
-        <v>0.025849057916375873</v>
+        <v>0.024035179897379078</v>
       </c>
     </row>
     <row r="56">
@@ -1215,10 +1212,10 @@
         <v>80</v>
       </c>
       <c r="C56" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D56" t="n">
-        <v>0.023940410195486816</v>
+        <v>0.02199462103004135</v>
       </c>
     </row>
     <row r="57">
@@ -1229,10 +1226,10 @@
         <v>81</v>
       </c>
       <c r="C57" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D57" t="n">
-        <v>0.021994384299169945</v>
+        <v>0.019957952290163616</v>
       </c>
     </row>
     <row r="58">
@@ -1243,10 +1240,10 @@
         <v>83</v>
       </c>
       <c r="C58" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D58" t="n">
-        <v>0.020044045712877323</v>
+        <v>0.017957499659263798</v>
       </c>
     </row>
     <row r="59">
@@ -1257,10 +1254,10 @@
         <v>84</v>
       </c>
       <c r="C59" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D59" t="n">
-        <v>0.018119754684082556</v>
+        <v>0.01602160954283749</v>
       </c>
     </row>
     <row r="60">
@@ -1271,10 +1268,10 @@
         <v>85</v>
       </c>
       <c r="C60" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D60" t="n">
-        <v>0.016248474612823582</v>
+        <v>0.01417414299235753</v>
       </c>
     </row>
     <row r="61">
@@ -1285,10 +1282,10 @@
         <v>87</v>
       </c>
       <c r="C61" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D61" t="n">
-        <v>0.014453273866616045</v>
+        <v>0.012434200478872948</v>
       </c>
     </row>
     <row r="62">
@@ -1299,10 +1296,10 @@
         <v>88</v>
       </c>
       <c r="C62" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D62" t="n">
-        <v>0.012753025283739616</v>
+        <v>0.010816065532932406</v>
       </c>
     </row>
     <row r="63">
@@ -1313,10 +1310,10 @@
         <v>89</v>
       </c>
       <c r="C63" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D63" t="n">
-        <v>0.011162296702602492</v>
+        <v>0.009329344778666426</v>
       </c>
     </row>
     <row r="64">
@@ -1327,10 +1324,10 @@
         <v>91</v>
       </c>
       <c r="C64" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D64" t="n">
-        <v>0.009691416454386537</v>
+        <v>0.007979273753471877</v>
       </c>
     </row>
     <row r="65">
@@ -1341,10 +1338,10 @@
         <v>92</v>
       </c>
       <c r="C65" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D65" t="n">
-        <v>0.00834669035744822</v>
+        <v>0.006767152678813563</v>
       </c>
     </row>
     <row r="66">
@@ -1355,10 +1352,10 @@
         <v>93</v>
       </c>
       <c r="C66" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D66" t="n">
-        <v>0.007130741627938725</v>
+        <v>0.005690874033349825</v>
       </c>
     </row>
     <row r="67">
@@ -1369,10 +1366,10 @@
         <v>95</v>
       </c>
       <c r="C67" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D67" t="n">
-        <v>0.006042942342825555</v>
+        <v>0.004745504151374782</v>
       </c>
     </row>
     <row r="68">
@@ -1383,10 +1380,10 @@
         <v>96</v>
       </c>
       <c r="C68" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D68" t="n">
-        <v>0.005079904546061012</v>
+        <v>0.003923883724839495</v>
       </c>
     </row>
     <row r="69">
@@ -1397,10 +1394,10 @@
         <v>97</v>
       </c>
       <c r="C69" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D69" t="n">
-        <v>0.004236000512180298</v>
+        <v>0.0032172165050838794</v>
       </c>
     </row>
     <row r="70">
@@ -1411,10 +1408,10 @@
         <v>99</v>
       </c>
       <c r="C70" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D70" t="n">
-        <v>0.003503884700880403</v>
+        <v>0.002615621103199059</v>
       </c>
     </row>
     <row r="71">
@@ -1425,10 +1422,10 @@
         <v>100</v>
       </c>
       <c r="C71" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D71" t="n">
-        <v>0.00287499411440594</v>
+        <v>0.00210862699870843</v>
       </c>
     </row>
     <row r="72">
@@ -1439,10 +1436,10 @@
         <v>101</v>
       </c>
       <c r="C72" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D72" t="n">
-        <v>0.0023400086511543242</v>
+        <v>0.0016856021568725224</v>
       </c>
     </row>
     <row r="73">
@@ -1453,10 +1450,10 @@
         <v>103</v>
       </c>
       <c r="C73" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D73" t="n">
-        <v>0.001889258198931829</v>
+        <v>0.0013361055821213335</v>
       </c>
     </row>
     <row r="74">
@@ -1467,10 +1464,10 @@
         <v>104</v>
       </c>
       <c r="C74" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D74" t="n">
-        <v>0.0015130682470696037</v>
+        <v>0.0010501633623933352</v>
       </c>
     </row>
     <row r="75">
@@ -1481,10 +1478,10 @@
         <v>105</v>
       </c>
       <c r="C75" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D75" t="n">
-        <v>0.0012020404095168134</v>
+        <v>8.184710652093417E-4</v>
       </c>
     </row>
     <row r="76">
@@ -1495,10 +1492,10 @@
         <v>107</v>
       </c>
       <c r="C76" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D76" t="n">
-        <v>9.472682180555812E-4</v>
+        <v>6.325286215140148E-4</v>
       </c>
     </row>
     <row r="77">
@@ -1509,10 +1506,10 @@
         <v>108</v>
       </c>
       <c r="C77" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D77" t="n">
-        <v>7.404917306698157E-4</v>
+        <v>4.8471606686904876E-4</v>
       </c>
     </row>
     <row r="78">
@@ -1523,10 +1520,10 @@
         <v>109</v>
       </c>
       <c r="C78" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D78" t="n">
-        <v>5.741968515153516E-4</v>
+        <v>3.6831977034729527E-4</v>
       </c>
     </row>
     <row r="79">
@@ -1537,10 +1534,10 @@
         <v>111</v>
       </c>
       <c r="C79" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D79" t="n">
-        <v>4.416667927248971E-4</v>
+        <v>2.77519195718153E-4</v>
       </c>
     </row>
     <row r="80">
@@ -1551,10 +1548,10 @@
         <v>112</v>
       </c>
       <c r="C80" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D80" t="n">
-        <v>3.3699389603134586E-4</v>
+        <v>2.0734396824795775E-4</v>
       </c>
     </row>
     <row r="81">
@@ -1565,52 +1562,52 @@
         <v>113</v>
       </c>
       <c r="C81" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D81" t="n">
-        <v>2.55060183311897E-4</v>
+        <v>1.5361023868065086E-4</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>54</v>
+        <v>114</v>
       </c>
       <c r="B82" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C82" t="s">
         <v>6</v>
       </c>
       <c r="D82" t="n">
-        <v>1.914946502662194E-4</v>
+        <v>1.1284421543794224E-4</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>54</v>
+        <v>114</v>
       </c>
       <c r="B83" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C83" t="s">
         <v>6</v>
       </c>
       <c r="D83" t="n">
-        <v>1.42614593609708E-4</v>
+        <v>8.219943220723778E-5</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>54</v>
+        <v>117</v>
       </c>
       <c r="B84" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C84" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="D84" t="n">
-        <v>1.0535730085837601E-4</v>
+        <v>5.937296151935681E-5</v>
       </c>
     </row>
     <row r="85">
@@ -1618,13 +1615,13 @@
         <v>117</v>
       </c>
       <c r="B85" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C85" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="D85" t="n">
-        <v>7.720735007968885E-5</v>
+        <v>4.2524477277995325E-5</v>
       </c>
     </row>
     <row r="86">
@@ -1632,27 +1629,27 @@
         <v>117</v>
       </c>
       <c r="B86" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C86" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="D86" t="n">
-        <v>5.612366203345721E-5</v>
+        <v>3.0200882409903937E-5</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B87" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C87" t="s">
         <v>6</v>
       </c>
       <c r="D87" t="n">
-        <v>4.0469393617832076E-5</v>
+        <v>2.1268196140727013E-5</v>
       </c>
     </row>
     <row r="88">
@@ -1660,41 +1657,13 @@
         <v>121</v>
       </c>
       <c r="B88" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C88" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D88" t="n">
-        <v>2.8946811650979124E-5</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="s">
-        <v>121</v>
-      </c>
-      <c r="B89" t="s">
-        <v>123</v>
-      </c>
-      <c r="C89" t="s">
-        <v>27</v>
-      </c>
-      <c r="D89" t="n">
-        <v>2.053847126341509E-5</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="s">
-        <v>121</v>
-      </c>
-      <c r="B90" t="s">
-        <v>124</v>
-      </c>
-      <c r="C90" t="s">
-        <v>27</v>
-      </c>
-      <c r="D90" t="n">
-        <v>1.4455357427856575E-5</v>
+        <v>1.4851559397829867E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>